<commit_message>
new hourly data thru early nov
</commit_message>
<xml_diff>
--- a/data/monitors_activity_full.xlsx
+++ b/data/monitors_activity_full.xlsx
@@ -439,6 +439,9 @@
       <c r="H2">
         <v>-117.379100757789</v>
       </c>
+      <c r="I2">
+        <v>1494</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3">
@@ -476,7 +479,7 @@
         <v>-117.43583467013</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4">
@@ -515,7 +518,7 @@
         <v>-117.43583467013</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="5">
@@ -554,7 +557,7 @@
         <v>-117.477866621737</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="6">
@@ -593,7 +596,7 @@
         <v>-117.477866621737</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="7">
@@ -632,7 +635,7 @@
         <v>-117.479946471589</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>3153</v>
       </c>
     </row>
     <row r="8">
@@ -671,7 +674,7 @@
         <v>-117.40844094425</v>
       </c>
       <c r="I8">
-        <v>3</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="9">
@@ -710,7 +713,7 @@
         <v>-117.405480924616</v>
       </c>
       <c r="I9">
-        <v>3</v>
+        <v>3174</v>
       </c>
     </row>
     <row r="10">
@@ -749,7 +752,7 @@
         <v>-117.422482970959</v>
       </c>
       <c r="I10">
-        <v>3</v>
+        <v>3150</v>
       </c>
     </row>
     <row r="11">
@@ -788,7 +791,7 @@
         <v>-117.460449334083</v>
       </c>
       <c r="I11">
-        <v>3</v>
+        <v>3002</v>
       </c>
     </row>
     <row r="12">
@@ -827,7 +830,7 @@
         <v>-117.401803200341</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13">
@@ -866,7 +869,7 @@
         <v>-117.401803200341</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14">
@@ -905,7 +908,7 @@
         <v>-117.479946471589</v>
       </c>
       <c r="I14">
-        <v>3</v>
+        <v>3438</v>
       </c>
     </row>
     <row r="15">
@@ -959,7 +962,7 @@
         <v>-117.374683262663</v>
       </c>
       <c r="I16">
-        <v>3</v>
+        <v>3585</v>
       </c>
     </row>
     <row r="17">
@@ -998,7 +1001,7 @@
         <v>-117.412833771021</v>
       </c>
       <c r="I17">
-        <v>3</v>
+        <v>3586</v>
       </c>
     </row>
     <row r="18">
@@ -1037,7 +1040,7 @@
         <v>-117.394816876874</v>
       </c>
       <c r="I18">
-        <v>3</v>
+        <v>3586</v>
       </c>
     </row>
     <row r="19">
@@ -1076,7 +1079,7 @@
         <v>-117.394816876874</v>
       </c>
       <c r="I19">
-        <v>3</v>
+        <v>3440</v>
       </c>
     </row>
     <row r="20">
@@ -1115,7 +1118,7 @@
         <v>-117.47946763197</v>
       </c>
       <c r="I20">
-        <v>3</v>
+        <v>3579</v>
       </c>
     </row>
     <row r="21">
@@ -1154,7 +1157,7 @@
         <v>-117.407539662333</v>
       </c>
       <c r="I21">
-        <v>3</v>
+        <v>3583</v>
       </c>
     </row>
     <row r="22">
@@ -1193,7 +1196,7 @@
         <v>-117.407539662333</v>
       </c>
       <c r="I22">
-        <v>4</v>
+        <v>3895</v>
       </c>
     </row>
     <row r="23">
@@ -1232,7 +1235,7 @@
         <v>-117.379100757789</v>
       </c>
       <c r="I23">
-        <v>4</v>
+        <v>3804</v>
       </c>
     </row>
     <row r="24">
@@ -1271,7 +1274,7 @@
         <v>-117.422482970959</v>
       </c>
       <c r="I24">
-        <v>4</v>
+        <v>4191</v>
       </c>
     </row>
     <row r="25">
@@ -1310,7 +1313,7 @@
         <v>-117.43649865802</v>
       </c>
       <c r="I25">
-        <v>5</v>
+        <v>3778</v>
       </c>
     </row>
     <row r="26">
@@ -1328,7 +1331,7 @@
         </is>
       </c>
       <c r="I26">
-        <v>2</v>
+        <v>827</v>
       </c>
     </row>
     <row r="27">
@@ -1367,7 +1370,7 @@
         <v>-117.363414880485</v>
       </c>
       <c r="I27">
-        <v>5</v>
+        <v>4303</v>
       </c>
     </row>
     <row r="28">
@@ -1385,7 +1388,7 @@
         </is>
       </c>
       <c r="I28">
-        <v>5</v>
+        <v>773</v>
       </c>
     </row>
     <row r="29">
@@ -1424,7 +1427,7 @@
         <v>-117.374683262663</v>
       </c>
       <c r="I29">
-        <v>5</v>
+        <v>4561</v>
       </c>
     </row>
     <row r="30">
@@ -1463,7 +1466,7 @@
         <v>-117.47946763197</v>
       </c>
       <c r="I30">
-        <v>5</v>
+        <v>4710</v>
       </c>
     </row>
     <row r="31">
@@ -1502,7 +1505,7 @@
         <v>-117.412833771021</v>
       </c>
       <c r="I31">
-        <v>5</v>
+        <v>4713</v>
       </c>
     </row>
     <row r="32">
@@ -1541,7 +1544,7 @@
         <v>-117.501099438453</v>
       </c>
       <c r="I32">
-        <v>4</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="33">
@@ -1579,6 +1582,9 @@
       <c r="H33">
         <v>-117.501099438453</v>
       </c>
+      <c r="I33">
+        <v>106</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34">
@@ -1616,7 +1622,7 @@
         <v>-117.4836</v>
       </c>
       <c r="I34">
-        <v>5</v>
+        <v>3672</v>
       </c>
     </row>
     <row r="35">
@@ -1633,6 +1639,9 @@
           <t>indoor</t>
         </is>
       </c>
+      <c r="I35">
+        <v>106</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36">
@@ -1670,7 +1679,7 @@
         <v>-117.389453648051</v>
       </c>
       <c r="I36">
-        <v>6</v>
+        <v>4405</v>
       </c>
     </row>
     <row r="37">
@@ -1709,7 +1718,7 @@
         <v>-117.389453648051</v>
       </c>
       <c r="I37">
-        <v>6</v>
+        <v>5618</v>
       </c>
     </row>
     <row r="38">
@@ -1748,7 +1757,7 @@
         <v>-117.400441932798</v>
       </c>
       <c r="I38">
-        <v>7</v>
+        <v>6410</v>
       </c>
     </row>
     <row r="39">
@@ -1787,7 +1796,7 @@
         <v>-117.400441932798</v>
       </c>
       <c r="I39">
-        <v>7</v>
+        <v>5405</v>
       </c>
     </row>
     <row r="40">
@@ -1826,7 +1835,7 @@
         <v>-117.398289631668</v>
       </c>
       <c r="I40">
-        <v>6</v>
+        <v>4289</v>
       </c>
     </row>
     <row r="41">
@@ -1865,7 +1874,7 @@
         <v>-117.398289631668</v>
       </c>
       <c r="I41">
-        <v>7</v>
+        <v>6411</v>
       </c>
     </row>
     <row r="42">
@@ -1904,7 +1913,7 @@
         <v>-117.480999262292</v>
       </c>
       <c r="I42">
-        <v>6</v>
+        <v>3965</v>
       </c>
     </row>
     <row r="43">
@@ -1943,7 +1952,7 @@
         <v>-117.480999262292</v>
       </c>
       <c r="I43">
-        <v>4</v>
+        <v>1768</v>
       </c>
     </row>
     <row r="44">
@@ -1982,7 +1991,7 @@
         <v>-117.395025416286</v>
       </c>
       <c r="I44">
-        <v>6</v>
+        <v>5076</v>
       </c>
     </row>
     <row r="45">
@@ -2021,7 +2030,7 @@
         <v>-117.395025416286</v>
       </c>
       <c r="I45">
-        <v>7</v>
+        <v>6429</v>
       </c>
     </row>
     <row r="46">
@@ -2075,7 +2084,7 @@
         <v>-117.493941090065</v>
       </c>
       <c r="I47">
-        <v>2</v>
+        <v>913</v>
       </c>
     </row>
     <row r="48">
@@ -2114,7 +2123,7 @@
         <v>-117.493941090065</v>
       </c>
       <c r="I48">
-        <v>7</v>
+        <v>6574</v>
       </c>
     </row>
     <row r="49">
@@ -2153,7 +2162,7 @@
         <v>-117.484178508747</v>
       </c>
       <c r="I49">
-        <v>7</v>
+        <v>6550</v>
       </c>
     </row>
     <row r="50">
@@ -2192,7 +2201,7 @@
         <v>-117.484178508747</v>
       </c>
       <c r="I50">
-        <v>7</v>
+        <v>6572</v>
       </c>
     </row>
     <row r="51">
@@ -2231,7 +2240,7 @@
         <v>-117.382571313447</v>
       </c>
       <c r="I51">
-        <v>7</v>
+        <v>6581</v>
       </c>
     </row>
     <row r="52">
@@ -2270,7 +2279,7 @@
         <v>-117.405480924616</v>
       </c>
       <c r="I52">
-        <v>7</v>
+        <v>5594</v>
       </c>
     </row>
     <row r="53">
@@ -2324,7 +2333,7 @@
         <v>-117.40844094425</v>
       </c>
       <c r="I54">
-        <v>5</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="55">
@@ -2363,7 +2372,7 @@
         <v>-117.402823108262</v>
       </c>
       <c r="I55">
-        <v>7</v>
+        <v>5974</v>
       </c>
     </row>
     <row r="56">
@@ -2402,7 +2411,7 @@
         <v>-117.396350795661</v>
       </c>
       <c r="I56">
-        <v>2</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="57">
@@ -2441,7 +2450,7 @@
         <v>-117.396350795661</v>
       </c>
       <c r="I57">
-        <v>1</v>
+        <v>616</v>
       </c>
     </row>
     <row r="58">
@@ -2480,7 +2489,7 @@
         <v>-117.448074055079</v>
       </c>
       <c r="I58">
-        <v>2</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="59">
@@ -2519,7 +2528,7 @@
         <v>-117.448074055079</v>
       </c>
       <c r="I59">
-        <v>5</v>
+        <v>4566</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
epic very salient plot!
</commit_message>
<xml_diff>
--- a/data/monitors_activity_full.xlsx
+++ b/data/monitors_activity_full.xlsx
@@ -439,6 +439,9 @@
       <c r="H2">
         <v>-117.379100757789</v>
       </c>
+      <c r="I2">
+        <v>1494</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3">
@@ -476,7 +479,7 @@
         <v>-117.43583467013</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4">
@@ -515,7 +518,7 @@
         <v>-117.43583467013</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="5">
@@ -554,7 +557,7 @@
         <v>-117.477866621737</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="6">
@@ -593,7 +596,7 @@
         <v>-117.477866621737</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="7">
@@ -632,7 +635,7 @@
         <v>-117.479946471589</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>3153</v>
       </c>
     </row>
     <row r="8">
@@ -671,7 +674,7 @@
         <v>-117.40844094425</v>
       </c>
       <c r="I8">
-        <v>3</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="9">
@@ -710,7 +713,7 @@
         <v>-117.405480924616</v>
       </c>
       <c r="I9">
-        <v>3</v>
+        <v>3174</v>
       </c>
     </row>
     <row r="10">
@@ -749,7 +752,7 @@
         <v>-117.422482970959</v>
       </c>
       <c r="I10">
-        <v>3</v>
+        <v>3150</v>
       </c>
     </row>
     <row r="11">
@@ -788,7 +791,7 @@
         <v>-117.460449334083</v>
       </c>
       <c r="I11">
-        <v>3</v>
+        <v>3002</v>
       </c>
     </row>
     <row r="12">
@@ -827,7 +830,7 @@
         <v>-117.401803200341</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13">
@@ -866,7 +869,7 @@
         <v>-117.401803200341</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14">
@@ -905,7 +908,7 @@
         <v>-117.479946471589</v>
       </c>
       <c r="I14">
-        <v>3</v>
+        <v>3438</v>
       </c>
     </row>
     <row r="15">
@@ -959,7 +962,7 @@
         <v>-117.374683262663</v>
       </c>
       <c r="I16">
-        <v>3</v>
+        <v>3585</v>
       </c>
     </row>
     <row r="17">
@@ -998,7 +1001,7 @@
         <v>-117.412833771021</v>
       </c>
       <c r="I17">
-        <v>3</v>
+        <v>3586</v>
       </c>
     </row>
     <row r="18">
@@ -1037,7 +1040,7 @@
         <v>-117.394816876874</v>
       </c>
       <c r="I18">
-        <v>3</v>
+        <v>3586</v>
       </c>
     </row>
     <row r="19">
@@ -1076,7 +1079,7 @@
         <v>-117.394816876874</v>
       </c>
       <c r="I19">
-        <v>3</v>
+        <v>3440</v>
       </c>
     </row>
     <row r="20">
@@ -1115,7 +1118,7 @@
         <v>-117.47946763197</v>
       </c>
       <c r="I20">
-        <v>3</v>
+        <v>3579</v>
       </c>
     </row>
     <row r="21">
@@ -1154,7 +1157,7 @@
         <v>-117.407539662333</v>
       </c>
       <c r="I21">
-        <v>3</v>
+        <v>3583</v>
       </c>
     </row>
     <row r="22">
@@ -1193,7 +1196,7 @@
         <v>-117.407539662333</v>
       </c>
       <c r="I22">
-        <v>4</v>
+        <v>3895</v>
       </c>
     </row>
     <row r="23">
@@ -1232,7 +1235,7 @@
         <v>-117.379100757789</v>
       </c>
       <c r="I23">
-        <v>4</v>
+        <v>3804</v>
       </c>
     </row>
     <row r="24">
@@ -1271,7 +1274,7 @@
         <v>-117.422482970959</v>
       </c>
       <c r="I24">
-        <v>4</v>
+        <v>4191</v>
       </c>
     </row>
     <row r="25">
@@ -1310,7 +1313,7 @@
         <v>-117.43649865802</v>
       </c>
       <c r="I25">
-        <v>5</v>
+        <v>3778</v>
       </c>
     </row>
     <row r="26">
@@ -1328,7 +1331,7 @@
         </is>
       </c>
       <c r="I26">
-        <v>2</v>
+        <v>827</v>
       </c>
     </row>
     <row r="27">
@@ -1367,7 +1370,7 @@
         <v>-117.363414880485</v>
       </c>
       <c r="I27">
-        <v>5</v>
+        <v>4303</v>
       </c>
     </row>
     <row r="28">
@@ -1385,7 +1388,7 @@
         </is>
       </c>
       <c r="I28">
-        <v>5</v>
+        <v>773</v>
       </c>
     </row>
     <row r="29">
@@ -1424,7 +1427,7 @@
         <v>-117.374683262663</v>
       </c>
       <c r="I29">
-        <v>5</v>
+        <v>4561</v>
       </c>
     </row>
     <row r="30">
@@ -1463,7 +1466,7 @@
         <v>-117.47946763197</v>
       </c>
       <c r="I30">
-        <v>5</v>
+        <v>4710</v>
       </c>
     </row>
     <row r="31">
@@ -1502,7 +1505,7 @@
         <v>-117.412833771021</v>
       </c>
       <c r="I31">
-        <v>5</v>
+        <v>4713</v>
       </c>
     </row>
     <row r="32">
@@ -1541,7 +1544,7 @@
         <v>-117.501099438453</v>
       </c>
       <c r="I32">
-        <v>4</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="33">
@@ -1579,6 +1582,9 @@
       <c r="H33">
         <v>-117.501099438453</v>
       </c>
+      <c r="I33">
+        <v>106</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34">
@@ -1616,7 +1622,7 @@
         <v>-117.4836</v>
       </c>
       <c r="I34">
-        <v>5</v>
+        <v>3672</v>
       </c>
     </row>
     <row r="35">
@@ -1633,6 +1639,9 @@
           <t>indoor</t>
         </is>
       </c>
+      <c r="I35">
+        <v>106</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36">
@@ -1670,7 +1679,7 @@
         <v>-117.389453648051</v>
       </c>
       <c r="I36">
-        <v>6</v>
+        <v>4405</v>
       </c>
     </row>
     <row r="37">
@@ -1709,7 +1718,7 @@
         <v>-117.389453648051</v>
       </c>
       <c r="I37">
-        <v>6</v>
+        <v>5618</v>
       </c>
     </row>
     <row r="38">
@@ -1748,7 +1757,7 @@
         <v>-117.400441932798</v>
       </c>
       <c r="I38">
-        <v>7</v>
+        <v>6410</v>
       </c>
     </row>
     <row r="39">
@@ -1787,7 +1796,7 @@
         <v>-117.400441932798</v>
       </c>
       <c r="I39">
-        <v>7</v>
+        <v>5405</v>
       </c>
     </row>
     <row r="40">
@@ -1826,7 +1835,7 @@
         <v>-117.398289631668</v>
       </c>
       <c r="I40">
-        <v>6</v>
+        <v>4289</v>
       </c>
     </row>
     <row r="41">
@@ -1865,7 +1874,7 @@
         <v>-117.398289631668</v>
       </c>
       <c r="I41">
-        <v>7</v>
+        <v>6411</v>
       </c>
     </row>
     <row r="42">
@@ -1904,7 +1913,7 @@
         <v>-117.480999262292</v>
       </c>
       <c r="I42">
-        <v>6</v>
+        <v>3965</v>
       </c>
     </row>
     <row r="43">
@@ -1943,7 +1952,7 @@
         <v>-117.480999262292</v>
       </c>
       <c r="I43">
-        <v>4</v>
+        <v>1768</v>
       </c>
     </row>
     <row r="44">
@@ -1982,7 +1991,7 @@
         <v>-117.395025416286</v>
       </c>
       <c r="I44">
-        <v>6</v>
+        <v>5076</v>
       </c>
     </row>
     <row r="45">
@@ -2021,7 +2030,7 @@
         <v>-117.395025416286</v>
       </c>
       <c r="I45">
-        <v>7</v>
+        <v>6429</v>
       </c>
     </row>
     <row r="46">
@@ -2075,7 +2084,7 @@
         <v>-117.493941090065</v>
       </c>
       <c r="I47">
-        <v>2</v>
+        <v>913</v>
       </c>
     </row>
     <row r="48">
@@ -2114,7 +2123,7 @@
         <v>-117.493941090065</v>
       </c>
       <c r="I48">
-        <v>7</v>
+        <v>6574</v>
       </c>
     </row>
     <row r="49">
@@ -2153,7 +2162,7 @@
         <v>-117.484178508747</v>
       </c>
       <c r="I49">
-        <v>7</v>
+        <v>6550</v>
       </c>
     </row>
     <row r="50">
@@ -2192,7 +2201,7 @@
         <v>-117.484178508747</v>
       </c>
       <c r="I50">
-        <v>7</v>
+        <v>6572</v>
       </c>
     </row>
     <row r="51">
@@ -2231,7 +2240,7 @@
         <v>-117.382571313447</v>
       </c>
       <c r="I51">
-        <v>7</v>
+        <v>6581</v>
       </c>
     </row>
     <row r="52">
@@ -2270,7 +2279,7 @@
         <v>-117.405480924616</v>
       </c>
       <c r="I52">
-        <v>7</v>
+        <v>5594</v>
       </c>
     </row>
     <row r="53">
@@ -2324,7 +2333,7 @@
         <v>-117.40844094425</v>
       </c>
       <c r="I54">
-        <v>5</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="55">
@@ -2363,7 +2372,7 @@
         <v>-117.402823108262</v>
       </c>
       <c r="I55">
-        <v>7</v>
+        <v>5974</v>
       </c>
     </row>
     <row r="56">
@@ -2402,7 +2411,7 @@
         <v>-117.396350795661</v>
       </c>
       <c r="I56">
-        <v>2</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="57">
@@ -2441,7 +2450,7 @@
         <v>-117.396350795661</v>
       </c>
       <c r="I57">
-        <v>1</v>
+        <v>616</v>
       </c>
     </row>
     <row r="58">
@@ -2480,7 +2489,7 @@
         <v>-117.448074055079</v>
       </c>
       <c r="I58">
-        <v>2</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="59">
@@ -2519,7 +2528,7 @@
         <v>-117.448074055079</v>
       </c>
       <c r="I59">
-        <v>5</v>
+        <v>4566</v>
       </c>
     </row>
   </sheetData>

</xml_diff>